<commit_message>
update part 1 excel file
</commit_message>
<xml_diff>
--- a/images/IntroExcelSampleWorkbook.xlsx
+++ b/images/IntroExcelSampleWorkbook.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="7665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$10</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Hire Date</t>
   </si>
@@ -122,18 +121,6 @@
   </si>
   <si>
     <t>Marvin Washington</t>
-  </si>
-  <si>
-    <t>College Degree</t>
-  </si>
-  <si>
-    <t>Professional development</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>Salesperson</t>
@@ -482,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -498,7 +485,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -975,551 +962,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>850</v>
-      </c>
-      <c r="D2">
-        <v>500</v>
-      </c>
-      <c r="E2" s="2">
-        <v>42373</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>950</v>
-      </c>
-      <c r="D3">
-        <v>475</v>
-      </c>
-      <c r="E3" s="2">
-        <v>43019</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-      <c r="D4">
-        <v>695</v>
-      </c>
-      <c r="E4" s="2">
-        <v>41672</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>400</v>
-      </c>
-      <c r="D5">
-        <v>700</v>
-      </c>
-      <c r="E5" s="2">
-        <v>40763</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <v>450</v>
-      </c>
-      <c r="E6" s="2">
-        <v>38721</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>1200</v>
-      </c>
-      <c r="D7">
-        <v>900</v>
-      </c>
-      <c r="E7" s="2">
-        <v>36623</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>250</v>
-      </c>
-      <c r="D8">
-        <v>575</v>
-      </c>
-      <c r="E8" s="2">
-        <v>36327</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>325</v>
-      </c>
-      <c r="D9">
-        <v>450</v>
-      </c>
-      <c r="E9" s="2">
-        <v>42265</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>1000</v>
-      </c>
-      <c r="D10">
-        <v>1000</v>
-      </c>
-      <c r="E10" s="2">
-        <v>41672</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>600</v>
-      </c>
-      <c r="D11">
-        <v>750</v>
-      </c>
-      <c r="E11" s="2">
-        <v>42829</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>1150</v>
-      </c>
-      <c r="D12">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="2">
-        <v>42987</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>900</v>
-      </c>
-      <c r="D13">
-        <v>850</v>
-      </c>
-      <c r="E13" s="2">
-        <v>41656</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>875</v>
-      </c>
-      <c r="D14">
-        <v>900</v>
-      </c>
-      <c r="E14" s="2">
-        <v>40415</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>1000</v>
-      </c>
-      <c r="D15">
-        <v>1150</v>
-      </c>
-      <c r="E15" s="2">
-        <v>39145</v>
-      </c>
-      <c r="F15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>1300</v>
-      </c>
-      <c r="D16">
-        <v>1000</v>
-      </c>
-      <c r="E16" s="2">
-        <v>36562</v>
-      </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>1250</v>
-      </c>
-      <c r="D17">
-        <v>1000</v>
-      </c>
-      <c r="E17" s="2">
-        <v>35931</v>
-      </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>545</v>
-      </c>
-      <c r="D18">
-        <v>550</v>
-      </c>
-      <c r="E18" s="2">
-        <v>42295</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>750</v>
-      </c>
-      <c r="D19">
-        <v>600</v>
-      </c>
-      <c r="E19" s="2">
-        <v>41677</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>1000</v>
-      </c>
-      <c r="D20">
-        <v>900</v>
-      </c>
-      <c r="E20" s="2">
-        <v>36713</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21">
-        <v>800</v>
-      </c>
-      <c r="D21">
-        <v>1100</v>
-      </c>
-      <c r="E21" s="2">
-        <v>35977</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>700</v>
-      </c>
-      <c r="D22">
-        <v>750</v>
-      </c>
-      <c r="E22" s="2">
-        <v>42356</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>450</v>
-      </c>
-      <c r="D23">
-        <v>650</v>
-      </c>
-      <c r="E23" s="2">
-        <v>41827</v>
-      </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>